<commit_message>
Upgrade to Sprint 21
Upgardes the alpha release source to the latest
sprint source (Sprint 21)
</commit_message>
<xml_diff>
--- a/changes-required/db-change-log.xlsx
+++ b/changes-required/db-change-log.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="61">
   <si>
     <t>Date Requested</t>
   </si>
@@ -138,6 +138,96 @@
   </si>
   <si>
     <t xml:space="preserve">Confirmed with Neil that the Despatch action should not cause a status change on the application. Only the Archive action updates the status to Completed. </t>
+  </si>
+  <si>
+    <t>application.application_status_type</t>
+  </si>
+  <si>
+    <t>Change display_value for the dead status to Annulled</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dead is not a good description for a status. Annulled / Annulment accurately reflects the state of the application does not have the negative conotations of Dead. Agreed with Neil. </t>
+  </si>
+  <si>
+    <t>Alexander</t>
+  </si>
+  <si>
+    <t>Add new role - "ManageBR" with displayValue="Manage business rules" and Description="Allows to manage business rules".</t>
+  </si>
+  <si>
+    <t>system.query_fields</t>
+  </si>
+  <si>
+    <t>Add field_name to query_fields table. Must be not null and match the name of the field used in the dynamic query.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MyBatis does necessarily  not return the query results in the order they are selected and omits null values completely from the reuslt Map. Need to use the field_name to match the returned values to there field display values.  </t>
+  </si>
+  <si>
+    <t>system.query_fields data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Mybatis code will merge the fields from query_fields with the fields in the query result to ensure all fields are included in the generic result. This minimises the configuration of query fields to only those that require localized display names. </t>
+  </si>
+  <si>
+    <t>system.query</t>
+  </si>
+  <si>
+    <t>Update all informationtool selects to use the_geom at the alias for st_asewkb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ensures  the field name used for st_asewkb in the Generic Result  is the_geom. This avoids the need for additional config in query_fields for this field. </t>
+  </si>
+  <si>
+    <t>Remove config data for the id field and the_geom field. Code now treats the values in query_fields as those requiring display names. All other fields in the query are obtained from the result set.  Ensure index is reordered from 0</t>
+  </si>
+  <si>
+    <t>Update informationtool . Get_application query to select nr as label rather than label</t>
+  </si>
+  <si>
+    <t xml:space="preserve">label does not exist in the application table. </t>
+  </si>
+  <si>
+    <t>Elton: I added column name instead of field_name, because I have used everywhere in db</t>
+  </si>
+  <si>
+    <t>We can also leave it nr in this case without putting as label.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Has to be changed to system.query_field </t>
+  </si>
+  <si>
+    <t>because everywhere in the db / model the naming is in singular</t>
+  </si>
+  <si>
+    <t>Everywhere</t>
+  </si>
+  <si>
+    <t>triggers to handle default values for columns that are not optional but supplied with nulls has to be removed.</t>
+  </si>
+  <si>
+    <t>This is handled in the service layer</t>
+  </si>
+  <si>
+    <t>party.is_rightholder</t>
+  </si>
+  <si>
+    <t>Return true if party connected with any RRR</t>
+  </si>
+  <si>
+    <t>Needed to distinguish parties as rightholders</t>
+  </si>
+  <si>
+    <t>CREATE OR REPLACE FUNCTION "party".is_rightholder(id character varying)
+  RETURNS boolean AS
+$BODY$
+BEGIN
+  return (SELECT (CASE (SELECT COUNT(1) FROM administrative.party_for_rrr ap WHERE ap.party_id = id) WHEN 0 THEN false ELSE true END));
+END;
+$BODY$
+  LANGUAGE plpgsql VOLATILE
+  COST 100;
+ALTER FUNCTION "party".is_rightholder(character varying) OWNER TO postgres;</t>
   </si>
 </sst>
 </file>
@@ -181,7 +271,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -199,6 +289,12 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -495,11 +591,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -684,6 +780,195 @@
       </c>
       <c r="E8" s="1" t="s">
         <v>33</v>
+      </c>
+      <c r="F8" s="8">
+        <v>40891</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="45">
+      <c r="A9" s="3">
+        <v>40879</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F9" s="8">
+        <v>40891</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="60">
+      <c r="A10" s="7">
+        <v>40884</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F10" s="8">
+        <v>40891</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="60">
+      <c r="A11" s="3">
+        <v>40891</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F11" s="8">
+        <v>40891</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="105">
+      <c r="A12" s="3">
+        <v>40891</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F12" s="8">
+        <v>40891</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="45">
+      <c r="A13" s="3">
+        <v>40891</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F13" s="8">
+        <v>40891</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="45">
+      <c r="A14" s="3">
+        <v>40891</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F14" s="8">
+        <v>40891</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="30">
+      <c r="A15" s="3">
+        <v>40891</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F15" s="8">
+        <v>40891</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="60">
+      <c r="A16" s="3">
+        <v>40891</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F16" s="8">
+        <v>40891</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="255">
+      <c r="A17" s="7">
+        <v>40891</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F17" s="8">
+        <v>40893</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>